<commit_message>
Update Frankfurt Melanoma plate metadata/layout
</commit_message>
<xml_diff>
--- a/Frankfurt_Melanoma/metadata/drug_plate_layout_1.0.xlsx
+++ b/Frankfurt_Melanoma/metadata/drug_plate_layout_1.0.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\Frankfurt\melanoma_DRP\plate_layout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A57FD0-C0B4-4E9C-A9F1-6B3A5C6A9CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="13185" yWindow="3690" windowWidth="23385" windowHeight="16410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,25 @@
     <sheet name="condition" sheetId="3" r:id="rId3"/>
     <sheet name="replicate" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="63">
   <si>
     <t>A</t>
   </si>
@@ -258,13 +277,29 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Temozolomide</t>
+  </si>
+  <si>
+    <t>Dacarbazine</t>
+  </si>
+  <si>
+    <t>1000x
+Temozolomide
+ 1</t>
+  </si>
+  <si>
+    <t>1000x
+Dacarbazine
+ 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,15 +316,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -312,11 +353,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -324,11 +378,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="12">
     <dxf>
       <border>
         <left style="medium">
@@ -373,15 +431,259 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color auto="1"/>
+        </left>
+        <right style="medium">
+          <color auto="1"/>
+        </right>
+        <top style="medium">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF32A879"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -419,7 +721,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -453,6 +755,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -487,9 +790,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -662,17 +966,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" customHeight="1">
+    <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -710,7 +1019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" customHeight="1">
+    <row r="2" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -720,6 +1029,9 @@
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
@@ -727,7 +1039,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" customHeight="1">
+    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -737,6 +1049,9 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
@@ -744,7 +1059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="60" customHeight="1">
+    <row r="4" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -761,7 +1076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" customHeight="1">
+    <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -778,7 +1093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60" customHeight="1">
+    <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -795,7 +1110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="60" customHeight="1">
+    <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -812,7 +1127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="60" customHeight="1">
+    <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -829,7 +1144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" customHeight="1">
+    <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -848,36 +1163,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="11" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="10" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M9">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="9" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" customHeight="1">
+    <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -915,7 +1233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" customHeight="1">
+    <row r="2" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -925,6 +1243,9 @@
       <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>41</v>
       </c>
@@ -932,7 +1253,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" customHeight="1">
+    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -942,6 +1263,9 @@
       <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>41</v>
       </c>
@@ -949,7 +1273,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="60" customHeight="1">
+    <row r="4" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -966,7 +1290,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" customHeight="1">
+    <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -983,7 +1307,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60" customHeight="1">
+    <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="60" customHeight="1">
+    <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1341,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="60" customHeight="1">
+    <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1358,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" customHeight="1">
+    <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1053,17 +1377,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="8" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="7" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M9">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="6" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1072,17 +1396,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" customHeight="1">
+    <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -1120,7 +1446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" customHeight="1">
+    <row r="2" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1130,6 +1456,9 @@
       <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>42</v>
       </c>
@@ -1137,7 +1466,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" customHeight="1">
+    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1147,6 +1476,9 @@
       <c r="C3" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1154,7 +1486,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="60" customHeight="1">
+    <row r="4" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1171,7 +1503,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" customHeight="1">
+    <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1188,7 +1520,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60" customHeight="1">
+    <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1537,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="60" customHeight="1">
+    <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1222,7 +1554,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="60" customHeight="1">
+    <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1239,7 +1571,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" customHeight="1">
+    <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1258,17 +1590,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="5" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M1">
-    <cfRule type="notContainsErrors" dxfId="1" priority="2">
+    <cfRule type="notContainsErrors" dxfId="4" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M9">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+    <cfRule type="notContainsErrors" dxfId="3" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1277,17 +1609,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="13" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" customHeight="1">
+    <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -1325,7 +1659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" customHeight="1">
+    <row r="2" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1335,6 +1669,9 @@
       <c r="C2" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1342,7 +1679,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" customHeight="1">
+    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1352,6 +1689,9 @@
       <c r="C3" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
       <c r="L3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1359,7 +1699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="60" customHeight="1">
+    <row r="4" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1716,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" customHeight="1">
+    <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1393,7 +1733,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60" customHeight="1">
+    <row r="6" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1410,7 +1750,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="60" customHeight="1">
+    <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1427,7 +1767,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="60" customHeight="1">
+    <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1444,7 +1784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" customHeight="1">
+    <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1803,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A9">
-    <cfRule type="notContainsErrors" dxfId="1" priority="3">
+    <cfRule type="notContainsErrors" dxfId="2" priority="3">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>